<commit_message>
Update challenges and quizzes
</commit_message>
<xml_diff>
--- a/backend/src/data/excel/challenges.xlsx
+++ b/backend/src/data/excel/challenges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nolan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C468844-C829-44BF-BCCC-D4EACBFF7669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0ED0FF-B19C-4B74-B297-6CCBE68A5813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39885" yWindow="4050" windowWidth="19110" windowHeight="11145" xr2:uid="{506E4E51-E7D9-4F5F-85A9-6ADE11E15C86}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -99,7 +99,25 @@
     <t>Steak Solana</t>
   </si>
   <si>
-    <t>Steak 3 solana coins</t>
+    <t>Stake 3 solana coins</t>
+  </si>
+  <si>
+    <t>Have 3 different coins in wallet</t>
+  </si>
+  <si>
+    <t>Have 6 different coins in wallet</t>
+  </si>
+  <si>
+    <t>Have 10 different coins in wallet</t>
+  </si>
+  <si>
+    <t>Coin Collector #1</t>
+  </si>
+  <si>
+    <t>Coin Collector #2</t>
+  </si>
+  <si>
+    <t>Coin Collector #3</t>
   </si>
 </sst>
 </file>
@@ -116,12 +134,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,8 +160,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697536E-C44D-45FD-8231-74D92DDC5F77}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,7 +505,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -494,7 +519,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -508,7 +533,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -522,7 +547,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -560,7 +585,7 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -574,7 +599,7 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -588,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -603,6 +628,48 @@
       </c>
       <c r="D10">
         <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix challenges table problem
</commit_message>
<xml_diff>
--- a/backend/src/data/excel/challenges.xlsx
+++ b/backend/src/data/excel/challenges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nolan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C522E3B-B555-4A45-B4E7-ACF3601DB542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085352AB-6FE6-4FED-B5BA-0FD7AA7F92A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{506E4E51-E7D9-4F5F-85A9-6ADE11E15C86}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{506E4E51-E7D9-4F5F-85A9-6ADE11E15C86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Welcome to Solasafe</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -448,20 +451,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697536E-C44D-45FD-8231-74D92DDC5F77}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.54296875" customWidth="1"/>
     <col min="3" max="3" width="32.90625" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +479,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -488,8 +496,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -502,8 +513,11 @@
       <c r="D3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -516,8 +530,11 @@
       <c r="D4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -530,8 +547,11 @@
       <c r="D5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -544,8 +564,11 @@
       <c r="D6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -558,27 +581,9 @@
       <c r="D7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
+      <c r="E7">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>